<commit_message>
ready to server telkom
</commit_message>
<xml_diff>
--- a/public/template/template_product_price.xlsx
+++ b/public/template/template_product_price.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INARTS-USER\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ampps\www\consys\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>lokasi</t>
-  </si>
-  <si>
     <t>harga_jasa</t>
   </si>
   <si>
@@ -36,6 +33,9 @@
   </si>
   <si>
     <t>jakarta</t>
+  </si>
+  <si>
+    <t>price_coverage</t>
   </si>
 </sst>
 </file>
@@ -357,28 +357,29 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>10000</v>

</xml_diff>